<commit_message>
add remaining Test scripts with expected status code add testng.xml file to run tests add docker image
</commit_message>
<xml_diff>
--- a/src/main/resources/Users-test-data.xlsx
+++ b/src/main/resources/Users-test-data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saeedsokar/Desktop/Saeed/Private/QPros-API/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C51A632-00EA-5544-A972-2CC91C3C0452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273E218D-8E6D-FB41-B81E-DEAEA6613404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{998C987E-4317-D240-BEDF-4297B69D2583}"/>
+    <workbookView xWindow="-32440" yWindow="1760" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{998C987E-4317-D240-BEDF-4297B69D2583}"/>
   </bookViews>
   <sheets>
     <sheet name="getUser" sheetId="1" r:id="rId1"/>
+    <sheet name="loginUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>user1</t>
   </si>
@@ -60,6 +61,24 @@
   </si>
   <si>
     <t>Dummy</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SD21@@!#D</t>
   </si>
 </sst>
 </file>
@@ -424,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EE9861-C342-8E41-8270-4499928C8E14}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -482,4 +501,88 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE645C3B-EB92-6542-9B44-235B63822EBA}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{18C6E9DA-48EE-A24C-843C-8E70F779CEF6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>